<commit_message>
Update Dockerfile and add more example sounds
</commit_message>
<xml_diff>
--- a/example/3s_Concat_FriCoe_TurPhi_TurMer.xlsx
+++ b/example/3s_Concat_FriCoe_TurPhi_TurMer.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="channel 1" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -446,2046 +446,2046 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Kohlmeise</t>
+          <t>Parus major</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Buchfink</t>
+          <t>Fringilla coelebs</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Nachtigall</t>
+          <t>Luscinia megarhynchos</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Amsel</t>
+          <t>Turdus merula</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Zilpzalp</t>
+          <t>Phylloscopus collybita</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Rotkehlchen</t>
+          <t>Erithacus rubecula</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Fitis</t>
+          <t>Phylloscopus trochilus</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Blaumeise</t>
+          <t>Cyanistes caeruleus</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Mönchsgrasmücke</t>
+          <t>Sylvia atricapilla</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Goldammer</t>
+          <t>Emberiza citrinella</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Singdrossel</t>
+          <t>Turdus philomelos</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Zaunkönig</t>
+          <t>Troglodytes troglodytes</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Dorngrasmücke</t>
+          <t>Sylvia communis</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Ortolan</t>
+          <t>Emberiza hortulana</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Tannenmeise</t>
+          <t>Periparus ater</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Grünfink</t>
+          <t>Chloris chloris</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Fichtenkreuzschnabel</t>
+          <t>Loxia curvirostra</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Buntspecht</t>
+          <t>Dendrocopos major</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Kleiber</t>
+          <t>Sitta europaea</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Grauammer</t>
+          <t>Emberiza calandra</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Baumpieper</t>
+          <t>Anthus trivialis</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Eichelhäher</t>
+          <t>Garrulus glandarius</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Feldlerche</t>
+          <t>Alauda arvensis</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Feldsperling</t>
+          <t>Passer montanus</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Gartenrotschwanz</t>
+          <t>Phoenicurus phoenicurus</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Schwanzmeise</t>
+          <t>Aegithalos caudatus</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>Rohrammer</t>
+          <t>Emberiza schoeniclus</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>Klappergrasmücke</t>
+          <t>Sylvia curruca</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>Heckenbraunelle</t>
+          <t>Prunella modularis</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>Gartengrasmücke</t>
+          <t>Sylvia borin</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>Wintergoldhähnchen</t>
+          <t>Regulus regulus</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>Stieglitz</t>
+          <t>Carduelis carduelis</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>Sumpfmeise</t>
+          <t>Poecile palustris</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>Haussperling</t>
+          <t>Passer domesticus</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>Schwarzspecht</t>
+          <t>Dryocopus martius</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>Gimpel</t>
+          <t>Pyrrhula pyrrhula</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>Wachtelkönig</t>
+          <t>Crex crex</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>Wacholderdrossel</t>
+          <t>Turdus pilaris</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>Sumpfrohrsänger</t>
+          <t>Acrocephalus palustris</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>Kolkrabe</t>
+          <t>Corvus corax</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>Weidenmeise</t>
+          <t>Poecile montanus</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>Waldkauz</t>
+          <t>Strix aluco</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>Teichrohrsänger</t>
+          <t>Acrocephalus scirpaceus</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>Kuckuck</t>
+          <t>Cuculus canorus</t>
         </is>
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>Gartenbaumläufer</t>
+          <t>Certhia brachydactyla</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>Samtkopf-Grasmücke</t>
+          <t>Sylvia melanocephala</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>Wasserralle</t>
+          <t>Rallus aquaticus</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
         <is>
-          <t>Haubenmeise</t>
+          <t>Lophophanes cristatus</t>
         </is>
       </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
-          <t>Seidensänger</t>
+          <t>Cettia cetti</t>
         </is>
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>Erlenzeisig</t>
+          <t>Carduelis spinus</t>
         </is>
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>Wiesenschafstelze</t>
+          <t>Motacilla flava</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
         <is>
-          <t>Waldbaumläufer</t>
+          <t>Certhia familiaris</t>
         </is>
       </c>
       <c r="BC1" s="1" t="inlineStr">
         <is>
-          <t>Misteldrossel</t>
+          <t>Turdus viscivorus</t>
         </is>
       </c>
       <c r="BD1" s="1" t="inlineStr">
         <is>
-          <t>Waldlaubsänger</t>
+          <t>Phylloscopus sibilatrix</t>
         </is>
       </c>
       <c r="BE1" s="1" t="inlineStr">
         <is>
-          <t>Bluthänfling</t>
+          <t>Carduelis cannabina</t>
         </is>
       </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
-          <t>Sprosser</t>
+          <t>Luscinia luscinia</t>
         </is>
       </c>
       <c r="BG1" s="1" t="inlineStr">
         <is>
-          <t>Schilfrohrsänger</t>
+          <t>Acrocephalus schoenobaenus</t>
         </is>
       </c>
       <c r="BH1" s="1" t="inlineStr">
         <is>
-          <t>Rauchschwalbe</t>
+          <t>Hirundo rustica</t>
         </is>
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>Trauerschnäpper</t>
+          <t>Ficedula hypoleuca</t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>Drosselrohrsänger</t>
+          <t>Acrocephalus arundinaceus</t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>Wiesenpieper</t>
+          <t>Anthus pratensis</t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
         <is>
-          <t>Star</t>
+          <t>Sturnus vulgaris</t>
         </is>
       </c>
       <c r="BM1" s="1" t="inlineStr">
         <is>
-          <t>Pirol</t>
+          <t>Oriolus oriolus</t>
         </is>
       </c>
       <c r="BN1" s="1" t="inlineStr">
         <is>
-          <t>Rotdrossel</t>
+          <t>Turdus iliacus</t>
         </is>
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>Bachstelze</t>
+          <t>Motacilla alba</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
         <is>
-          <t>Girlitz</t>
+          <t>Serinus serinus</t>
         </is>
       </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>Rabenkrähe</t>
+          <t>Corvus corone</t>
         </is>
       </c>
       <c r="BR1" s="1" t="inlineStr">
         <is>
-          <t>Kernbeißer</t>
+          <t>Coccothraustes coccothraustes</t>
         </is>
       </c>
       <c r="BS1" s="1" t="inlineStr">
         <is>
-          <t>Elster</t>
+          <t>Pica pica</t>
         </is>
       </c>
       <c r="BT1" s="1" t="inlineStr">
         <is>
-          <t>Sommergoldhähnchen</t>
+          <t>Regulus ignicapilla</t>
         </is>
       </c>
       <c r="BU1" s="1" t="inlineStr">
         <is>
-          <t>Karmingimpel</t>
+          <t>Carpodacus erythrinus</t>
         </is>
       </c>
       <c r="BV1" s="1" t="inlineStr">
         <is>
-          <t>Gelbspötter</t>
+          <t>Hippolais icterina</t>
         </is>
       </c>
       <c r="BW1" s="1" t="inlineStr">
         <is>
-          <t>Nebelkrähe</t>
+          <t>Corvus cornix</t>
         </is>
       </c>
       <c r="BX1" s="1" t="inlineStr">
         <is>
-          <t>Kleinspecht</t>
+          <t>Dendrocopos minor</t>
         </is>
       </c>
       <c r="BY1" s="1" t="inlineStr">
         <is>
-          <t>Blässhuhn</t>
+          <t>Fulica atra</t>
         </is>
       </c>
       <c r="BZ1" s="1" t="inlineStr">
         <is>
-          <t>Grünspecht</t>
+          <t>Picus viridis</t>
         </is>
       </c>
       <c r="CA1" s="1" t="inlineStr">
         <is>
-          <t>Iberienzilpzalp</t>
+          <t>Phylloscopus ibericus</t>
         </is>
       </c>
       <c r="CB1" s="1" t="inlineStr">
         <is>
-          <t>Hausrotschwanz</t>
+          <t>Phoenicurus ochruros</t>
         </is>
       </c>
       <c r="CC1" s="1" t="inlineStr">
         <is>
-          <t>Berglaubsänger</t>
+          <t>Phylloscopus bonelli</t>
         </is>
       </c>
       <c r="CD1" s="1" t="inlineStr">
         <is>
-          <t>Blaukehlchen</t>
+          <t>Luscinia svecica</t>
         </is>
       </c>
       <c r="CE1" s="1" t="inlineStr">
         <is>
-          <t>Stockente</t>
+          <t>Anas platyrhynchos</t>
         </is>
       </c>
       <c r="CF1" s="1" t="inlineStr">
         <is>
-          <t>Graugans</t>
+          <t>Anser anser</t>
         </is>
       </c>
       <c r="CG1" s="1" t="inlineStr">
         <is>
-          <t>Feldschwirl</t>
+          <t>Locustella naevia</t>
         </is>
       </c>
       <c r="CH1" s="1" t="inlineStr">
         <is>
-          <t>Tüpfelsumpfhuhn</t>
+          <t>Porzana porzana</t>
         </is>
       </c>
       <c r="CI1" s="1" t="inlineStr">
         <is>
-          <t>Bekassine</t>
+          <t>Gallinago gallinago</t>
         </is>
       </c>
       <c r="CJ1" s="1" t="inlineStr">
         <is>
-          <t>Heidelerche</t>
+          <t>Lullula arborea</t>
         </is>
       </c>
       <c r="CK1" s="1" t="inlineStr">
         <is>
-          <t>Rotschenkel</t>
+          <t>Tringa totanus</t>
         </is>
       </c>
       <c r="CL1" s="1" t="inlineStr">
         <is>
-          <t>Kiebitz</t>
+          <t>Vanellus vanellus</t>
         </is>
       </c>
       <c r="CM1" s="1" t="inlineStr">
         <is>
-          <t>Teichhuhn</t>
+          <t>Gallinula chloropus</t>
         </is>
       </c>
       <c r="CN1" s="1" t="inlineStr">
         <is>
-          <t>Braunkehlchen</t>
+          <t>Saxicola rubetra</t>
         </is>
       </c>
       <c r="CO1" s="1" t="inlineStr">
         <is>
-          <t>Großer Brachvogel</t>
+          <t>Numenius arquata</t>
         </is>
       </c>
       <c r="CP1" s="1" t="inlineStr">
         <is>
-          <t>Ziegenmelker</t>
+          <t>Caprimulgus europaeus</t>
         </is>
       </c>
       <c r="CQ1" s="1" t="inlineStr">
         <is>
-          <t>Mittelspecht</t>
+          <t>Dendrocopos medius</t>
         </is>
       </c>
       <c r="CR1" s="1" t="inlineStr">
         <is>
-          <t>Zaunammer</t>
+          <t>Emberiza cirlus</t>
         </is>
       </c>
       <c r="CS1" s="1" t="inlineStr">
         <is>
-          <t>Graureiher</t>
+          <t>Ardea cinerea</t>
         </is>
       </c>
       <c r="CT1" s="1" t="inlineStr">
         <is>
-          <t>Grauspecht</t>
+          <t>Picus canus</t>
         </is>
       </c>
       <c r="CU1" s="1" t="inlineStr">
         <is>
-          <t>Mäusebussard</t>
+          <t>Buteo buteo</t>
         </is>
       </c>
       <c r="CV1" s="1" t="inlineStr">
         <is>
-          <t>Zwergschnäpper</t>
+          <t>Ficedula parva</t>
         </is>
       </c>
       <c r="CW1" s="1" t="inlineStr">
         <is>
-          <t>Schlagschwirl</t>
+          <t>Locustella fluviatilis</t>
         </is>
       </c>
       <c r="CX1" s="1" t="inlineStr">
         <is>
-          <t>Lachmöwe</t>
+          <t>Chroicocephalus ridibundus</t>
         </is>
       </c>
       <c r="CY1" s="1" t="inlineStr">
         <is>
-          <t>Bergfink</t>
+          <t>Fringilla montifringilla</t>
         </is>
       </c>
       <c r="CZ1" s="1" t="inlineStr">
         <is>
-          <t>Dohle</t>
+          <t>Coloeus monedula</t>
         </is>
       </c>
       <c r="DA1" s="1" t="inlineStr">
         <is>
-          <t>Türkentaube</t>
+          <t>Streptopelia decaocto</t>
         </is>
       </c>
       <c r="DB1" s="1" t="inlineStr">
         <is>
-          <t>Grauschnäpper</t>
+          <t>Muscicapa striata</t>
         </is>
       </c>
       <c r="DC1" s="1" t="inlineStr">
         <is>
-          <t>Ringeltaube</t>
+          <t>Columba palumbus</t>
         </is>
       </c>
       <c r="DD1" s="1" t="inlineStr">
         <is>
-          <t>Saatkrähe</t>
+          <t>Corvus frugilegus</t>
         </is>
       </c>
       <c r="DE1" s="1" t="inlineStr">
         <is>
-          <t>Austernfischer</t>
+          <t>Haematopus ostralegus</t>
         </is>
       </c>
       <c r="DF1" s="1" t="inlineStr">
         <is>
-          <t>Mauersegler</t>
+          <t>Apus apus</t>
         </is>
       </c>
       <c r="DG1" s="1" t="inlineStr">
         <is>
-          <t>Kranich</t>
+          <t>Grus grus</t>
         </is>
       </c>
       <c r="DH1" s="1" t="inlineStr">
         <is>
-          <t>Waldohreule</t>
+          <t>Asio otus</t>
         </is>
       </c>
       <c r="DI1" s="1" t="inlineStr">
         <is>
-          <t>Jagdfasan</t>
+          <t>Phasianus colchicus</t>
         </is>
       </c>
       <c r="DJ1" s="1" t="inlineStr">
         <is>
-          <t>Raufußkauz</t>
+          <t>Aegolius funereus</t>
         </is>
       </c>
       <c r="DK1" s="1" t="inlineStr">
         <is>
-          <t>Sperbergrasmücke</t>
+          <t>Sylvia nisoria</t>
         </is>
       </c>
       <c r="DL1" s="1" t="inlineStr">
         <is>
-          <t>Bienenfresser</t>
+          <t>Merops apiaster</t>
         </is>
       </c>
       <c r="DM1" s="1" t="inlineStr">
         <is>
-          <t>Grünlaubsänger</t>
+          <t>Phylloscopus trochiloides</t>
         </is>
       </c>
       <c r="DN1" s="1" t="inlineStr">
         <is>
-          <t>Wachtel</t>
+          <t>Coturnix coturnix</t>
         </is>
       </c>
       <c r="DO1" s="1" t="inlineStr">
         <is>
-          <t>Birkenzeisig</t>
+          <t>Carduelis flammea</t>
         </is>
       </c>
       <c r="DP1" s="1" t="inlineStr">
         <is>
-          <t>Mehlschwalbe</t>
+          <t>Delichon urbicum</t>
         </is>
       </c>
       <c r="DQ1" s="1" t="inlineStr">
         <is>
-          <t>Haubenlerche</t>
+          <t>Galerida cristata</t>
         </is>
       </c>
       <c r="DR1" s="1" t="inlineStr">
         <is>
-          <t>Sturmmöwe</t>
+          <t>Larus canus</t>
         </is>
       </c>
       <c r="DS1" s="1" t="inlineStr">
         <is>
-          <t>Wiedehopf</t>
+          <t>Upupa epops</t>
         </is>
       </c>
       <c r="DT1" s="1" t="inlineStr">
         <is>
-          <t>Zwergtaucher</t>
+          <t>Tachybaptus ruficollis</t>
         </is>
       </c>
       <c r="DU1" s="1" t="inlineStr">
         <is>
-          <t>Wendehals</t>
+          <t>Jynx torquilla</t>
         </is>
       </c>
       <c r="DV1" s="1" t="inlineStr">
         <is>
-          <t>Rohrschwirl</t>
+          <t>Locustella luscinioides</t>
         </is>
       </c>
       <c r="DW1" s="1" t="inlineStr">
         <is>
-          <t>Tannenhäher</t>
+          <t>Nucifraga caryocatactes</t>
         </is>
       </c>
       <c r="DX1" s="1" t="inlineStr">
         <is>
-          <t>Grünschenkel</t>
+          <t>Tringa nebularia</t>
         </is>
       </c>
       <c r="DY1" s="1" t="inlineStr">
         <is>
-          <t>Zistensänger</t>
+          <t>Cisticola juncidis</t>
         </is>
       </c>
       <c r="DZ1" s="1" t="inlineStr">
         <is>
-          <t>Flussuferläufer</t>
+          <t>Actitis hypoleucos</t>
         </is>
       </c>
       <c r="EA1" s="1" t="inlineStr">
         <is>
-          <t>Schwarzkehlchen</t>
+          <t>Saxicola rubicola</t>
         </is>
       </c>
       <c r="EB1" s="1" t="inlineStr">
         <is>
-          <t>Eisvogel</t>
+          <t>Alcedo atthis</t>
         </is>
       </c>
       <c r="EC1" s="1" t="inlineStr">
         <is>
-          <t>Rohrdommel</t>
+          <t>Botaurus stellaris</t>
         </is>
       </c>
       <c r="ED1" s="1" t="inlineStr">
         <is>
-          <t>Waldschnepfe</t>
+          <t>Scolopax rusticola</t>
         </is>
       </c>
       <c r="EE1" s="1" t="inlineStr">
         <is>
-          <t>Zwergohreule</t>
+          <t>Otus scops</t>
         </is>
       </c>
       <c r="EF1" s="1" t="inlineStr">
         <is>
-          <t>Neuntöter</t>
+          <t>Lanius collurio</t>
         </is>
       </c>
       <c r="EG1" s="1" t="inlineStr">
         <is>
-          <t>Steinkauz</t>
+          <t>Athene noctua</t>
         </is>
       </c>
       <c r="EH1" s="1" t="inlineStr">
         <is>
-          <t>Uhu</t>
+          <t>Bubo bubo</t>
         </is>
       </c>
       <c r="EI1" s="1" t="inlineStr">
         <is>
-          <t>Singschwan</t>
+          <t>Cygnus cygnus</t>
         </is>
       </c>
       <c r="EJ1" s="1" t="inlineStr">
         <is>
-          <t>Kleines Sumpfhuhn</t>
+          <t>Porzana parva</t>
         </is>
       </c>
       <c r="EK1" s="1" t="inlineStr">
         <is>
-          <t>Höckerschwan</t>
+          <t>Cygnus olor</t>
         </is>
       </c>
       <c r="EL1" s="1" t="inlineStr">
         <is>
-          <t>Beutelmeise</t>
+          <t>Remiz pendulinus</t>
         </is>
       </c>
       <c r="EM1" s="1" t="inlineStr">
         <is>
-          <t>Flussregenpfeifer</t>
+          <t>Charadrius dubius</t>
         </is>
       </c>
       <c r="EN1" s="1" t="inlineStr">
         <is>
-          <t>Gebirgsstelze</t>
+          <t>Motacilla cinerea</t>
         </is>
       </c>
       <c r="EO1" s="1" t="inlineStr">
         <is>
-          <t>Waldwasserläufer</t>
+          <t>Tringa ochropus</t>
         </is>
       </c>
       <c r="EP1" s="1" t="inlineStr">
         <is>
-          <t>Uferschnepfe</t>
+          <t>Limosa limosa</t>
         </is>
       </c>
       <c r="EQ1" s="1" t="inlineStr">
         <is>
-          <t>Bruchwasserläufer</t>
+          <t>Tringa glareola</t>
         </is>
       </c>
       <c r="ER1" s="1" t="inlineStr">
         <is>
-          <t>Flussseeschwalbe</t>
+          <t>Sterna hirundo</t>
         </is>
       </c>
       <c r="ES1" s="1" t="inlineStr">
         <is>
-          <t>Weißbart-Grasmücke</t>
+          <t>Sylvia cantillans</t>
         </is>
       </c>
       <c r="ET1" s="1" t="inlineStr">
         <is>
-          <t>Silbermöwe</t>
+          <t>Larus argentatus</t>
         </is>
       </c>
       <c r="EU1" s="1" t="inlineStr">
         <is>
-          <t>Provencegrasmücke</t>
+          <t>Sylvia undata</t>
         </is>
       </c>
       <c r="EV1" s="1" t="inlineStr">
         <is>
-          <t>Turteltaube</t>
+          <t>Streptopelia turtur</t>
         </is>
       </c>
       <c r="EW1" s="1" t="inlineStr">
         <is>
-          <t>Halsbandschnäpper</t>
+          <t>Ficedula albicollis</t>
         </is>
       </c>
       <c r="EX1" s="1" t="inlineStr">
         <is>
-          <t>Blässgans</t>
+          <t>Anser albifrons</t>
         </is>
       </c>
       <c r="EY1" s="1" t="inlineStr">
         <is>
-          <t>Kanadagans</t>
+          <t>Branta canadensis</t>
         </is>
       </c>
       <c r="EZ1" s="1" t="inlineStr">
         <is>
-          <t>Kanarenzilpzalp</t>
+          <t>Phylloscopus canariensis</t>
         </is>
       </c>
       <c r="FA1" s="1" t="inlineStr">
         <is>
-          <t>Stelzenläufer</t>
+          <t>Himantopus himantopus</t>
         </is>
       </c>
       <c r="FB1" s="1" t="inlineStr">
         <is>
-          <t>Säbelschnäbler</t>
+          <t>Recurvirostra avosetta</t>
         </is>
       </c>
       <c r="FC1" s="1" t="inlineStr">
         <is>
-          <t>Rebhuhn</t>
+          <t>Perdix perdix</t>
         </is>
       </c>
       <c r="FD1" s="1" t="inlineStr">
         <is>
-          <t>Weißwangengans</t>
+          <t>Branta leucopsis</t>
         </is>
       </c>
       <c r="FE1" s="1" t="inlineStr">
         <is>
-          <t>Rothuhn</t>
+          <t>Alectoris rufa</t>
         </is>
       </c>
       <c r="FF1" s="1" t="inlineStr">
         <is>
-          <t>Steinschmätzer</t>
+          <t>Oenanthe oenanthe</t>
         </is>
       </c>
       <c r="FG1" s="1" t="inlineStr">
         <is>
-          <t>Bartmeise</t>
+          <t>Panurus biarmicus</t>
         </is>
       </c>
       <c r="FH1" s="1" t="inlineStr">
         <is>
-          <t>Haubentaucher</t>
+          <t>Podiceps cristatus</t>
         </is>
       </c>
       <c r="FI1" s="1" t="inlineStr">
         <is>
-          <t>Habicht</t>
+          <t>Accipiter gentilis</t>
         </is>
       </c>
       <c r="FJ1" s="1" t="inlineStr">
         <is>
-          <t>Pfeifente</t>
+          <t>Anas penelope</t>
         </is>
       </c>
       <c r="FK1" s="1" t="inlineStr">
         <is>
-          <t>Kiefernkreuzschnabel</t>
+          <t>Loxia pytyopsittacus</t>
         </is>
       </c>
       <c r="FL1" s="1" t="inlineStr">
         <is>
-          <t>Strandpieper</t>
+          <t>Anthus petrosus</t>
         </is>
       </c>
       <c r="FM1" s="1" t="inlineStr">
         <is>
-          <t>Bergpieper</t>
+          <t>Anthus spinoletta</t>
         </is>
       </c>
       <c r="FN1" s="1" t="inlineStr">
         <is>
-          <t>Mittelmeermöwe</t>
+          <t>Larus michahellis</t>
         </is>
       </c>
       <c r="FO1" s="1" t="inlineStr">
         <is>
-          <t>Uferschwalbe</t>
+          <t>Riparia riparia</t>
         </is>
       </c>
       <c r="FP1" s="1" t="inlineStr">
         <is>
-          <t>Rothalstaucher</t>
+          <t>Podiceps grisegena</t>
         </is>
       </c>
       <c r="FQ1" s="1" t="inlineStr">
         <is>
-          <t>Brachpieper</t>
+          <t>Anthus campestris</t>
         </is>
       </c>
       <c r="FR1" s="1" t="inlineStr">
         <is>
-          <t>Bindenkreuzschnabel</t>
+          <t>Loxia leucoptera</t>
         </is>
       </c>
       <c r="FS1" s="1" t="inlineStr">
         <is>
-          <t>Weißbart-Seeschwalbe</t>
+          <t>Chlidonias hybrida</t>
         </is>
       </c>
       <c r="FT1" s="1" t="inlineStr">
         <is>
-          <t>Turmfalke</t>
+          <t>Falco tinnunculus</t>
         </is>
       </c>
       <c r="FU1" s="1" t="inlineStr">
         <is>
-          <t>Zippammer</t>
+          <t>Emberiza cia</t>
         </is>
       </c>
       <c r="FV1" s="1" t="inlineStr">
         <is>
-          <t>Spornammer</t>
+          <t>Calcarius lapponicus</t>
         </is>
       </c>
       <c r="FW1" s="1" t="inlineStr">
         <is>
-          <t>Rotkehlpieper</t>
+          <t>Anthus cervinus</t>
         </is>
       </c>
       <c r="FX1" s="1" t="inlineStr">
         <is>
-          <t>Brandgans</t>
+          <t>Tadorna tadorna</t>
         </is>
       </c>
       <c r="FY1" s="1" t="inlineStr">
         <is>
-          <t>Rohrweihe</t>
+          <t>Circus aeruginosus</t>
         </is>
       </c>
       <c r="FZ1" s="1" t="inlineStr">
         <is>
-          <t>Haselhuhn</t>
+          <t>Tetrastes bonasia</t>
         </is>
       </c>
       <c r="GA1" s="1" t="inlineStr">
         <is>
-          <t>Schellente</t>
+          <t>Bucephala clangula</t>
         </is>
       </c>
       <c r="GB1" s="1" t="inlineStr">
         <is>
-          <t>Dunkler Wasserläufer</t>
+          <t>Tringa erythropus</t>
         </is>
       </c>
       <c r="GC1" s="1" t="inlineStr">
         <is>
-          <t>Kormoran</t>
+          <t>Phalacrocorax carbo</t>
         </is>
       </c>
       <c r="GD1" s="1" t="inlineStr">
         <is>
-          <t>Waldammer</t>
+          <t>Emberiza rustica</t>
         </is>
       </c>
       <c r="GE1" s="1" t="inlineStr">
         <is>
-          <t>Sandregenpfeifer</t>
+          <t>Charadrius hiaticula</t>
         </is>
       </c>
       <c r="GF1" s="1" t="inlineStr">
         <is>
-          <t>Schleiereule</t>
+          <t>Tyto alba</t>
         </is>
       </c>
       <c r="GG1" s="1" t="inlineStr">
         <is>
-          <t>Zwergdommel</t>
+          <t>Ixobrychus minutus</t>
         </is>
       </c>
       <c r="GH1" s="1" t="inlineStr">
         <is>
-          <t>Hohltaube</t>
+          <t>Columba oenas</t>
         </is>
       </c>
       <c r="GI1" s="1" t="inlineStr">
         <is>
-          <t>Raubwürger</t>
+          <t>Lanius excubitor</t>
         </is>
       </c>
       <c r="GJ1" s="1" t="inlineStr">
         <is>
-          <t>Reiherente</t>
+          <t>Aythya fuligula</t>
         </is>
       </c>
       <c r="GK1" s="1" t="inlineStr">
         <is>
-          <t>Weidensperling</t>
+          <t>Passer hispaniolensis</t>
         </is>
       </c>
       <c r="GL1" s="1" t="inlineStr">
         <is>
-          <t>Birkhuhn</t>
+          <t>Lyrurus tetrix</t>
         </is>
       </c>
       <c r="GM1" s="1" t="inlineStr">
         <is>
-          <t>Baumfalke</t>
+          <t>Falco subbuteo</t>
         </is>
       </c>
       <c r="GN1" s="1" t="inlineStr">
         <is>
-          <t>Regenbrachvogel</t>
+          <t>Numenius phaeopus</t>
         </is>
       </c>
       <c r="GO1" s="1" t="inlineStr">
         <is>
-          <t>Alpenstrandläufer</t>
+          <t>Calidris alpina</t>
         </is>
       </c>
       <c r="GP1" s="1" t="inlineStr">
         <is>
-          <t>Mantelmöwe</t>
+          <t>Larus marinus</t>
         </is>
       </c>
       <c r="GQ1" s="1" t="inlineStr">
         <is>
-          <t>Alpenkrähe</t>
+          <t>Pyrrhocorax pyrrhocorax</t>
         </is>
       </c>
       <c r="GR1" s="1" t="inlineStr">
         <is>
-          <t>Kalanderlerche</t>
+          <t>Melanocorypha calandra</t>
         </is>
       </c>
       <c r="GS1" s="1" t="inlineStr">
         <is>
-          <t>Schneeammer</t>
+          <t>Plectrophenax nivalis</t>
         </is>
       </c>
       <c r="GT1" s="1" t="inlineStr">
         <is>
-          <t>Zwergammer</t>
+          <t>Emberiza pusilla</t>
         </is>
       </c>
       <c r="GU1" s="1" t="inlineStr">
         <is>
-          <t>Tafelente</t>
+          <t>Aythya ferina</t>
         </is>
       </c>
       <c r="GV1" s="1" t="inlineStr">
         <is>
-          <t>Schnatterente</t>
+          <t>Anas strepera</t>
         </is>
       </c>
       <c r="GW1" s="1" t="inlineStr">
         <is>
-          <t>Küstenseeschwalbe</t>
+          <t>Sterna paradisaea</t>
         </is>
       </c>
       <c r="GX1" s="1" t="inlineStr">
         <is>
-          <t>Steinwälzer</t>
+          <t>Arenaria interpres</t>
         </is>
       </c>
       <c r="GY1" s="1" t="inlineStr">
         <is>
-          <t>Trauerseeschwalbe</t>
+          <t>Chlidonias niger</t>
         </is>
       </c>
       <c r="GZ1" s="1" t="inlineStr">
         <is>
-          <t>Heringsmöwe</t>
+          <t>Larus fuscus</t>
         </is>
       </c>
       <c r="HA1" s="1" t="inlineStr">
         <is>
-          <t>Wanderlaubsänger</t>
+          <t>Phylloscopus borealis</t>
         </is>
       </c>
       <c r="HB1" s="1" t="inlineStr">
         <is>
-          <t>Weißflügel-Seeschwalbe</t>
+          <t>Chlidonias leucopterus</t>
         </is>
       </c>
       <c r="HC1" s="1" t="inlineStr">
         <is>
-          <t>Blaumerle</t>
+          <t>Monticola solitarius</t>
         </is>
       </c>
       <c r="HD1" s="1" t="inlineStr">
         <is>
-          <t>Zitronenzeisig</t>
+          <t>Carduelis citrinella</t>
         </is>
       </c>
       <c r="HE1" s="1" t="inlineStr">
         <is>
-          <t>Brandseeschwalbe</t>
+          <t>Thalasseus sandvicensis</t>
         </is>
       </c>
       <c r="HF1" s="1" t="inlineStr">
         <is>
-          <t>Knäkente</t>
+          <t>Anas querquedula</t>
         </is>
       </c>
       <c r="HG1" s="1" t="inlineStr">
         <is>
-          <t>Seeadler</t>
+          <t>Haliaeetus albicilla</t>
         </is>
       </c>
       <c r="HH1" s="1" t="inlineStr">
         <is>
-          <t>Brillengrasmücke</t>
+          <t>Sylvia conspicillata</t>
         </is>
       </c>
       <c r="HI1" s="1" t="inlineStr">
         <is>
-          <t>Eiderente</t>
+          <t>Somateria mollissima</t>
         </is>
       </c>
       <c r="HJ1" s="1" t="inlineStr">
         <is>
-          <t>Theklalerche</t>
+          <t>Galerida theklae</t>
         </is>
       </c>
       <c r="HK1" s="1" t="inlineStr">
         <is>
-          <t>Seggenrohrsänger</t>
+          <t>Acrocephalus paludicola</t>
         </is>
       </c>
       <c r="HL1" s="1" t="inlineStr">
         <is>
-          <t>Zwergsumpfhuhn</t>
+          <t>Porzana pusilla</t>
         </is>
       </c>
       <c r="HM1" s="1" t="inlineStr">
         <is>
-          <t>Steppenmöwe</t>
+          <t>Larus cachinnans</t>
         </is>
       </c>
       <c r="HN1" s="1" t="inlineStr">
         <is>
-          <t>Seeregenpfeifer</t>
+          <t>Charadrius alexandrinus</t>
         </is>
       </c>
       <c r="HO1" s="1" t="inlineStr">
         <is>
-          <t>Sperber</t>
+          <t>Accipiter nisus</t>
         </is>
       </c>
       <c r="HP1" s="1" t="inlineStr">
         <is>
-          <t>Schwarzmilan</t>
+          <t>Milvus migrans</t>
         </is>
       </c>
       <c r="HQ1" s="1" t="inlineStr">
         <is>
-          <t>Alpendohle</t>
+          <t>Pyrrhocorax graculus</t>
         </is>
       </c>
       <c r="HR1" s="1" t="inlineStr">
         <is>
-          <t>Kurzzehenlerche</t>
+          <t>Calandrella brachydactyla</t>
         </is>
       </c>
       <c r="HS1" s="1" t="inlineStr">
         <is>
-          <t>Eisente</t>
+          <t>Clangula hyemalis</t>
         </is>
       </c>
       <c r="HT1" s="1" t="inlineStr">
         <is>
-          <t>Mariskenrohrsänger</t>
+          <t>Acrocephalus melanopogon</t>
         </is>
       </c>
       <c r="HU1" s="1" t="inlineStr">
         <is>
-          <t>Auerhuhn</t>
+          <t>Tetrao urogallus</t>
         </is>
       </c>
       <c r="HV1" s="1" t="inlineStr">
         <is>
-          <t>Nilgans</t>
+          <t>Alopochen aegyptiaca</t>
         </is>
       </c>
       <c r="HW1" s="1" t="inlineStr">
         <is>
-          <t>Prachttaucher</t>
+          <t>Gavia arctica</t>
         </is>
       </c>
       <c r="HX1" s="1" t="inlineStr">
         <is>
-          <t>Rosaflamingo</t>
+          <t>Phoenicopterus roseus</t>
         </is>
       </c>
       <c r="HY1" s="1" t="inlineStr">
         <is>
-          <t>Schneeeule</t>
+          <t>Bubo scandiacus</t>
         </is>
       </c>
       <c r="HZ1" s="1" t="inlineStr">
         <is>
-          <t>Wanderfalke</t>
+          <t>Falco peregrinus</t>
         </is>
       </c>
       <c r="IA1" s="1" t="inlineStr">
         <is>
-          <t>Stummellerche</t>
+          <t>Calandrella rufescens</t>
         </is>
       </c>
       <c r="IB1" s="1" t="inlineStr">
         <is>
-          <t>Kappenammer</t>
+          <t>Emberiza melanocephala</t>
         </is>
       </c>
       <c r="IC1" s="1" t="inlineStr">
         <is>
-          <t>Weidenammer</t>
+          <t>Emberiza aureola</t>
         </is>
       </c>
       <c r="ID1" s="1" t="inlineStr">
         <is>
-          <t>Saatgans</t>
+          <t>Anser fabalis</t>
         </is>
       </c>
       <c r="IE1" s="1" t="inlineStr">
         <is>
-          <t>Mornellregenpfeifer</t>
+          <t>Charadrius morinellus</t>
         </is>
       </c>
       <c r="IF1" s="1" t="inlineStr">
         <is>
-          <t>Fischadler</t>
+          <t>Pandion haliaetus</t>
         </is>
       </c>
       <c r="IG1" s="1" t="inlineStr">
         <is>
-          <t>Dreizehenmöwe</t>
+          <t>Rissa tridactyla</t>
         </is>
       </c>
       <c r="IH1" s="1" t="inlineStr">
         <is>
-          <t>Tundrasaatgans</t>
+          <t>Anser serrirostris</t>
         </is>
       </c>
       <c r="II1" s="1" t="inlineStr">
         <is>
-          <t>Schwarzhalstaucher</t>
+          <t>Podiceps nigricollis</t>
         </is>
       </c>
       <c r="IJ1" s="1" t="inlineStr">
         <is>
-          <t>Pfeifschwan, Zwergschwan</t>
+          <t>Cygnus columbianus</t>
         </is>
       </c>
       <c r="IK1" s="1" t="inlineStr">
         <is>
-          <t>Häherkuckuck</t>
+          <t>Clamator glandarius</t>
         </is>
       </c>
       <c r="IL1" s="1" t="inlineStr">
         <is>
-          <t>Sichelstrandläufer</t>
+          <t>Calidris ferruginea</t>
         </is>
       </c>
       <c r="IM1" s="1" t="inlineStr">
         <is>
-          <t>Alpenschneehuhn</t>
+          <t>Lagopus muta</t>
         </is>
       </c>
       <c r="IN1" s="1" t="inlineStr">
         <is>
-          <t>Rotmilan</t>
+          <t>Milvus milvus</t>
         </is>
       </c>
       <c r="IO1" s="1" t="inlineStr">
         <is>
-          <t>Schreiadler</t>
+          <t>Aquila pomarina</t>
         </is>
       </c>
       <c r="IP1" s="1" t="inlineStr">
         <is>
-          <t>Spießente</t>
+          <t>Anas acuta</t>
         </is>
       </c>
       <c r="IQ1" s="1" t="inlineStr">
         <is>
-          <t>Mittelsäger</t>
+          <t>Mergus serrator</t>
         </is>
       </c>
       <c r="IR1" s="1" t="inlineStr">
         <is>
-          <t>Knutt</t>
+          <t>Calidris canutus</t>
         </is>
       </c>
       <c r="IS1" s="1" t="inlineStr">
         <is>
-          <t>Skua</t>
+          <t>Stercorarius skua</t>
         </is>
       </c>
       <c r="IT1" s="1" t="inlineStr">
         <is>
-          <t>Olivenspötter</t>
+          <t>Hippolais olivetorum</t>
         </is>
       </c>
       <c r="IU1" s="1" t="inlineStr">
         <is>
-          <t>Trauersteinschmätzer</t>
+          <t>Oenanthe leucura</t>
         </is>
       </c>
       <c r="IV1" s="1" t="inlineStr">
         <is>
-          <t>Schwarzstirnwürger</t>
+          <t>Lanius minor</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05092</v>
+        <v>0.0204</v>
       </c>
       <c r="D2" t="n">
-        <v>0.05367</v>
+        <v>0.78011</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05022</v>
+        <v>0.08251</v>
       </c>
       <c r="F2" t="n">
-        <v>0.12865</v>
+        <v>0.68762</v>
       </c>
       <c r="G2" t="n">
-        <v>0.02859</v>
+        <v>0.03054</v>
       </c>
       <c r="H2" t="n">
-        <v>0.03835</v>
+        <v>0.04302</v>
       </c>
       <c r="I2" t="n">
-        <v>0.03675</v>
+        <v>0.03733</v>
       </c>
       <c r="J2" t="n">
-        <v>0.02444</v>
+        <v>0.0162</v>
       </c>
       <c r="K2" t="n">
-        <v>0.04408</v>
+        <v>0.06937</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0392</v>
+        <v>0.0424</v>
       </c>
       <c r="M2" t="n">
-        <v>0.71932</v>
+        <v>0.20055</v>
       </c>
       <c r="N2" t="n">
-        <v>0.02674</v>
+        <v>0.02802</v>
       </c>
       <c r="O2" t="n">
-        <v>0.02603</v>
+        <v>0.02337</v>
       </c>
       <c r="P2" t="n">
-        <v>0.03202</v>
+        <v>0.02652</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.01599</v>
+        <v>0.01249</v>
       </c>
       <c r="R2" t="n">
-        <v>0.02701</v>
+        <v>0.02907</v>
       </c>
       <c r="S2" t="n">
-        <v>0.02734</v>
+        <v>0.01356</v>
       </c>
       <c r="T2" t="n">
-        <v>0.02583</v>
+        <v>0.02281</v>
       </c>
       <c r="U2" t="n">
-        <v>0.03945</v>
+        <v>0.0236</v>
       </c>
       <c r="V2" t="n">
-        <v>0.02575</v>
+        <v>0.0234</v>
       </c>
       <c r="W2" t="n">
-        <v>0.02339</v>
+        <v>0.03298</v>
       </c>
       <c r="X2" t="n">
-        <v>0.02908</v>
+        <v>0.03998</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.02763</v>
+        <v>0.0179</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.02356</v>
+        <v>0.0163</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.01739</v>
+        <v>0.01982</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.01725</v>
+        <v>0.01419</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.01917</v>
+        <v>0.01249</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.02226</v>
+        <v>0.022</v>
       </c>
       <c r="AE2" t="n">
+        <v>0.02061</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.03521</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.00878</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.01314</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.0174</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.02397</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.03557</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.02303</v>
+      </c>
+      <c r="AM2" t="n">
         <v>0.02346</v>
       </c>
-      <c r="AF2" t="n">
-        <v>0.02202</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.01256</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>0.02356</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0.01748</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0.0426</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>0.02605</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0.02335</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.03534</v>
-      </c>
       <c r="AN2" t="n">
-        <v>0.03322</v>
+        <v>0.03493</v>
       </c>
       <c r="AO2" t="n">
+        <v>0.008959999999999999</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.0169</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.0179</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.01011</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.0092</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.0152</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.01639</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0.01326</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.01546</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0.01486</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>0.02273</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0.01123</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0.00616</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.01228</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0.03466</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0.02248</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0.01646</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0.02462</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0.00971</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.01222</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0.01678</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>0.01435</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0.01134</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0.03588</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0.01967</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>0.02215</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>0.01476</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>0.01075</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>0.01846</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>0.009860000000000001</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>0.01487</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>0.00882</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>0.01424</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>0.01061</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>0.00517</v>
+      </c>
+      <c r="BX2" t="n">
+        <v>0.01374</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>0.00773</v>
+      </c>
+      <c r="BZ2" t="n">
+        <v>0.01543</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>0.00814</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>0.01142</v>
+      </c>
+      <c r="CC2" t="n">
+        <v>0.01596</v>
+      </c>
+      <c r="CD2" t="n">
+        <v>0.00784</v>
+      </c>
+      <c r="CE2" t="n">
+        <v>0.0143</v>
+      </c>
+      <c r="CF2" t="n">
+        <v>0.01356</v>
+      </c>
+      <c r="CG2" t="n">
+        <v>0.01463</v>
+      </c>
+      <c r="CH2" t="n">
+        <v>0.01712</v>
+      </c>
+      <c r="CI2" t="n">
+        <v>0.00752</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>0.01237</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>0.01687</v>
+      </c>
+      <c r="CL2" t="n">
+        <v>0.01096</v>
+      </c>
+      <c r="CM2" t="n">
+        <v>0.01096</v>
+      </c>
+      <c r="CN2" t="n">
+        <v>0.01255</v>
+      </c>
+      <c r="CO2" t="n">
+        <v>0.00651</v>
+      </c>
+      <c r="CP2" t="n">
+        <v>0.01318</v>
+      </c>
+      <c r="CQ2" t="n">
+        <v>0.01665</v>
+      </c>
+      <c r="CR2" t="n">
+        <v>0.01841</v>
+      </c>
+      <c r="CS2" t="n">
+        <v>0.01178</v>
+      </c>
+      <c r="CT2" t="n">
+        <v>0.0102</v>
+      </c>
+      <c r="CU2" t="n">
+        <v>0.03162</v>
+      </c>
+      <c r="CV2" t="n">
         <v>0.02481</v>
       </c>
-      <c r="AP2" t="n">
-        <v>0.0243</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.018</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>0.01776</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>0.01336</v>
-      </c>
-      <c r="AT2" t="n">
-        <v>0.01562</v>
-      </c>
-      <c r="AU2" t="n">
-        <v>0.01622</v>
-      </c>
-      <c r="AV2" t="n">
-        <v>0.01451</v>
-      </c>
-      <c r="AW2" t="n">
-        <v>0.02664</v>
-      </c>
-      <c r="AX2" t="n">
-        <v>0.01359</v>
-      </c>
-      <c r="AY2" t="n">
-        <v>0.01545</v>
-      </c>
-      <c r="AZ2" t="n">
-        <v>0.01195</v>
-      </c>
-      <c r="BA2" t="n">
-        <v>0.01422</v>
-      </c>
-      <c r="BB2" t="n">
-        <v>0.01664</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>0.03505</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>0.01361</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>0.03153</v>
-      </c>
-      <c r="BF2" t="n">
-        <v>0.05035</v>
-      </c>
-      <c r="BG2" t="n">
-        <v>0.0124</v>
-      </c>
-      <c r="BH2" t="n">
-        <v>0.01374</v>
-      </c>
-      <c r="BI2" t="n">
-        <v>0.01633</v>
-      </c>
-      <c r="BJ2" t="n">
-        <v>0.01773</v>
-      </c>
-      <c r="BK2" t="n">
-        <v>0.01295</v>
-      </c>
-      <c r="BL2" t="n">
-        <v>0.02979</v>
-      </c>
-      <c r="BM2" t="n">
-        <v>0.02431</v>
-      </c>
-      <c r="BN2" t="n">
-        <v>0.02083</v>
-      </c>
-      <c r="BO2" t="n">
-        <v>0.01428</v>
-      </c>
-      <c r="BP2" t="n">
-        <v>0.01773</v>
-      </c>
-      <c r="BQ2" t="n">
-        <v>0.01304</v>
-      </c>
-      <c r="BR2" t="n">
-        <v>0.01257</v>
-      </c>
-      <c r="BS2" t="n">
-        <v>0.02484</v>
-      </c>
-      <c r="BT2" t="n">
-        <v>0.01458</v>
-      </c>
-      <c r="BU2" t="n">
-        <v>0.01574</v>
-      </c>
-      <c r="BV2" t="n">
-        <v>0.01838</v>
-      </c>
-      <c r="BW2" t="n">
-        <v>0.00923</v>
-      </c>
-      <c r="BX2" t="n">
-        <v>0.01585</v>
-      </c>
-      <c r="BY2" t="n">
-        <v>0.01314</v>
-      </c>
-      <c r="BZ2" t="n">
-        <v>0.02646</v>
-      </c>
-      <c r="CA2" t="n">
-        <v>0.008750000000000001</v>
-      </c>
-      <c r="CB2" t="n">
-        <v>0.01591</v>
-      </c>
-      <c r="CC2" t="n">
-        <v>0.01184</v>
-      </c>
-      <c r="CD2" t="n">
-        <v>0.02084</v>
-      </c>
-      <c r="CE2" t="n">
-        <v>0.0292</v>
-      </c>
-      <c r="CF2" t="n">
-        <v>0.01112</v>
-      </c>
-      <c r="CG2" t="n">
+      <c r="CW2" t="n">
+        <v>0.01719</v>
+      </c>
+      <c r="CX2" t="n">
+        <v>0.00796</v>
+      </c>
+      <c r="CY2" t="n">
+        <v>0.01602</v>
+      </c>
+      <c r="CZ2" t="n">
+        <v>0.00984</v>
+      </c>
+      <c r="DA2" t="n">
+        <v>0.00241</v>
+      </c>
+      <c r="DB2" t="n">
+        <v>0.01157</v>
+      </c>
+      <c r="DC2" t="n">
+        <v>0.009560000000000001</v>
+      </c>
+      <c r="DD2" t="n">
+        <v>0.01101</v>
+      </c>
+      <c r="DE2" t="n">
+        <v>0.01089</v>
+      </c>
+      <c r="DF2" t="n">
+        <v>0.00601</v>
+      </c>
+      <c r="DG2" t="n">
+        <v>0.00269</v>
+      </c>
+      <c r="DH2" t="n">
+        <v>0.00502</v>
+      </c>
+      <c r="DI2" t="n">
+        <v>0.007849999999999999</v>
+      </c>
+      <c r="DJ2" t="n">
+        <v>0.00518</v>
+      </c>
+      <c r="DK2" t="n">
+        <v>0.01122</v>
+      </c>
+      <c r="DL2" t="n">
+        <v>0.008970000000000001</v>
+      </c>
+      <c r="DM2" t="n">
+        <v>0.01241</v>
+      </c>
+      <c r="DN2" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="DO2" t="n">
+        <v>0.00572</v>
+      </c>
+      <c r="DP2" t="n">
+        <v>0.00477</v>
+      </c>
+      <c r="DQ2" t="n">
+        <v>0.0066</v>
+      </c>
+      <c r="DR2" t="n">
+        <v>0.00544</v>
+      </c>
+      <c r="DS2" t="n">
+        <v>0.00355</v>
+      </c>
+      <c r="DT2" t="n">
+        <v>0.00605</v>
+      </c>
+      <c r="DU2" t="n">
+        <v>0.0121</v>
+      </c>
+      <c r="DV2" t="n">
+        <v>0.01845</v>
+      </c>
+      <c r="DW2" t="n">
+        <v>0.01151</v>
+      </c>
+      <c r="DX2" t="n">
+        <v>0.01152</v>
+      </c>
+      <c r="DY2" t="n">
+        <v>0.01489</v>
+      </c>
+      <c r="DZ2" t="n">
+        <v>0.01064</v>
+      </c>
+      <c r="EA2" t="n">
+        <v>0.00389</v>
+      </c>
+      <c r="EB2" t="n">
+        <v>0.00459</v>
+      </c>
+      <c r="EC2" t="n">
+        <v>0.00124</v>
+      </c>
+      <c r="ED2" t="n">
+        <v>0.00821</v>
+      </c>
+      <c r="EE2" t="n">
+        <v>0.00362</v>
+      </c>
+      <c r="EF2" t="n">
+        <v>0.0167</v>
+      </c>
+      <c r="EG2" t="n">
+        <v>0.00366</v>
+      </c>
+      <c r="EH2" t="n">
+        <v>0.0057</v>
+      </c>
+      <c r="EI2" t="n">
+        <v>0.00184</v>
+      </c>
+      <c r="EJ2" t="n">
+        <v>0.00609</v>
+      </c>
+      <c r="EK2" t="n">
+        <v>0.0043</v>
+      </c>
+      <c r="EL2" t="n">
+        <v>0.00607</v>
+      </c>
+      <c r="EM2" t="n">
+        <v>0.00387</v>
+      </c>
+      <c r="EN2" t="n">
+        <v>0.009849999999999999</v>
+      </c>
+      <c r="EO2" t="n">
+        <v>0.00392</v>
+      </c>
+      <c r="EP2" t="n">
+        <v>0.00758</v>
+      </c>
+      <c r="EQ2" t="n">
         <v>0.00812</v>
       </c>
-      <c r="CH2" t="n">
-        <v>0.0159</v>
-      </c>
-      <c r="CI2" t="n">
-        <v>0.01244</v>
-      </c>
-      <c r="CJ2" t="n">
-        <v>0.01547</v>
-      </c>
-      <c r="CK2" t="n">
-        <v>0.01266</v>
-      </c>
-      <c r="CL2" t="n">
-        <v>0.01088</v>
-      </c>
-      <c r="CM2" t="n">
-        <v>0.01344</v>
-      </c>
-      <c r="CN2" t="n">
-        <v>0.01411</v>
-      </c>
-      <c r="CO2" t="n">
-        <v>0.01045</v>
-      </c>
-      <c r="CP2" t="n">
-        <v>0.0147</v>
-      </c>
-      <c r="CQ2" t="n">
-        <v>0.01661</v>
-      </c>
-      <c r="CR2" t="n">
-        <v>0.01323</v>
-      </c>
-      <c r="CS2" t="n">
-        <v>0.01069</v>
-      </c>
-      <c r="CT2" t="n">
-        <v>0.01617</v>
-      </c>
-      <c r="CU2" t="n">
-        <v>0.01426</v>
-      </c>
-      <c r="CV2" t="n">
-        <v>0.0205</v>
-      </c>
-      <c r="CW2" t="n">
-        <v>0.01685</v>
-      </c>
-      <c r="CX2" t="n">
-        <v>0.011</v>
-      </c>
-      <c r="CY2" t="n">
-        <v>0.01482</v>
-      </c>
-      <c r="CZ2" t="n">
-        <v>0.01986</v>
-      </c>
-      <c r="DA2" t="n">
-        <v>0.00423</v>
-      </c>
-      <c r="DB2" t="n">
-        <v>0.009849999999999999</v>
-      </c>
-      <c r="DC2" t="n">
-        <v>0.01365</v>
-      </c>
-      <c r="DD2" t="n">
-        <v>0.01337</v>
-      </c>
-      <c r="DE2" t="n">
-        <v>0.01386</v>
-      </c>
-      <c r="DF2" t="n">
-        <v>0.01273</v>
-      </c>
-      <c r="DG2" t="n">
-        <v>0.0106</v>
-      </c>
-      <c r="DH2" t="n">
-        <v>0.00817</v>
-      </c>
-      <c r="DI2" t="n">
-        <v>0.01107</v>
-      </c>
-      <c r="DJ2" t="n">
-        <v>0.02482</v>
-      </c>
-      <c r="DK2" t="n">
-        <v>0.01533</v>
-      </c>
-      <c r="DL2" t="n">
-        <v>0.01168</v>
-      </c>
-      <c r="DM2" t="n">
-        <v>0.008410000000000001</v>
-      </c>
-      <c r="DN2" t="n">
-        <v>0.01369</v>
-      </c>
-      <c r="DO2" t="n">
-        <v>0.00861</v>
-      </c>
-      <c r="DP2" t="n">
-        <v>0.01016</v>
-      </c>
-      <c r="DQ2" t="n">
-        <v>0.009860000000000001</v>
-      </c>
-      <c r="DR2" t="n">
-        <v>0.009429999999999999</v>
-      </c>
-      <c r="DS2" t="n">
-        <v>0.00385</v>
-      </c>
-      <c r="DT2" t="n">
-        <v>0.01325</v>
-      </c>
-      <c r="DU2" t="n">
-        <v>0.01604</v>
-      </c>
-      <c r="DV2" t="n">
-        <v>0.01643</v>
-      </c>
-      <c r="DW2" t="n">
-        <v>0.02256</v>
-      </c>
-      <c r="DX2" t="n">
-        <v>0.01102</v>
-      </c>
-      <c r="DY2" t="n">
-        <v>0.01326</v>
-      </c>
-      <c r="DZ2" t="n">
-        <v>0.01286</v>
-      </c>
-      <c r="EA2" t="n">
-        <v>0.00891</v>
-      </c>
-      <c r="EB2" t="n">
-        <v>0.00784</v>
-      </c>
-      <c r="EC2" t="n">
-        <v>0.00467</v>
-      </c>
-      <c r="ED2" t="n">
-        <v>0.01845</v>
-      </c>
-      <c r="EE2" t="n">
-        <v>0.0032</v>
-      </c>
-      <c r="EF2" t="n">
-        <v>0.01212</v>
-      </c>
-      <c r="EG2" t="n">
-        <v>0.00502</v>
-      </c>
-      <c r="EH2" t="n">
-        <v>0.00499</v>
-      </c>
-      <c r="EI2" t="n">
-        <v>0.0039</v>
-      </c>
-      <c r="EJ2" t="n">
-        <v>0.00882</v>
-      </c>
-      <c r="EK2" t="n">
-        <v>0.01015</v>
-      </c>
-      <c r="EL2" t="n">
-        <v>0.00658</v>
-      </c>
-      <c r="EM2" t="n">
-        <v>0.009719999999999999</v>
-      </c>
-      <c r="EN2" t="n">
-        <v>0.00971</v>
-      </c>
-      <c r="EO2" t="n">
-        <v>0.008959999999999999</v>
-      </c>
-      <c r="EP2" t="n">
-        <v>0.00651</v>
-      </c>
-      <c r="EQ2" t="n">
-        <v>0.01356</v>
-      </c>
       <c r="ER2" t="n">
-        <v>0.0078</v>
+        <v>0.00732</v>
       </c>
       <c r="ES2" t="n">
-        <v>0.00517</v>
+        <v>0.00492</v>
       </c>
       <c r="ET2" t="n">
-        <v>0.00366</v>
+        <v>0.00219</v>
       </c>
       <c r="EU2" t="n">
-        <v>0.00596</v>
+        <v>0.00822</v>
       </c>
       <c r="EV2" t="n">
-        <v>0.00735</v>
+        <v>0.00234</v>
       </c>
       <c r="EW2" t="n">
-        <v>0.01209</v>
+        <v>0.01027</v>
       </c>
       <c r="EX2" t="n">
-        <v>0.00649</v>
+        <v>0.00404</v>
       </c>
       <c r="EY2" t="n">
-        <v>0.00265</v>
+        <v>0.0014</v>
       </c>
       <c r="EZ2" t="n">
-        <v>0.0052</v>
+        <v>0.00595</v>
       </c>
       <c r="FA2" t="n">
-        <v>0.00545</v>
+        <v>0.00298</v>
       </c>
       <c r="FB2" t="n">
-        <v>0.00632</v>
+        <v>0.00512</v>
       </c>
       <c r="FC2" t="n">
-        <v>0.00533</v>
+        <v>0.00512</v>
       </c>
       <c r="FD2" t="n">
-        <v>0.00617</v>
+        <v>0.00399</v>
       </c>
       <c r="FE2" t="n">
-        <v>0.00589</v>
+        <v>0.00524</v>
       </c>
       <c r="FF2" t="n">
-        <v>0.00812</v>
+        <v>0.00337</v>
       </c>
       <c r="FG2" t="n">
-        <v>0.00765</v>
+        <v>0.00557</v>
       </c>
       <c r="FH2" t="n">
-        <v>0.0031</v>
+        <v>0.00094</v>
       </c>
       <c r="FI2" t="n">
-        <v>0.007849999999999999</v>
+        <v>0.00684</v>
       </c>
       <c r="FJ2" t="n">
-        <v>0.00654</v>
+        <v>0.00611</v>
       </c>
       <c r="FK2" t="n">
-        <v>0.01009</v>
+        <v>0.00743</v>
       </c>
       <c r="FL2" t="n">
-        <v>0.00944</v>
+        <v>0.00371</v>
       </c>
       <c r="FM2" t="n">
         <v>0.00751</v>
       </c>
       <c r="FN2" t="n">
-        <v>0.00187</v>
+        <v>0.00151</v>
       </c>
       <c r="FO2" t="n">
-        <v>0.00649</v>
+        <v>0.00637</v>
       </c>
       <c r="FP2" t="n">
-        <v>0.00389</v>
+        <v>0.0029</v>
       </c>
       <c r="FQ2" t="n">
-        <v>0.01055</v>
+        <v>0.00588</v>
       </c>
       <c r="FR2" t="n">
-        <v>0.009860000000000001</v>
+        <v>0.00349</v>
       </c>
       <c r="FS2" t="n">
-        <v>0.01053</v>
+        <v>0.00439</v>
       </c>
       <c r="FT2" t="n">
-        <v>0.00663</v>
+        <v>0.00595</v>
       </c>
       <c r="FU2" t="n">
-        <v>0.0072</v>
+        <v>0.00642</v>
       </c>
       <c r="FV2" t="n">
-        <v>0.01228</v>
+        <v>0.00795</v>
       </c>
       <c r="FW2" t="n">
-        <v>0.00596</v>
+        <v>0.00288</v>
       </c>
       <c r="FX2" t="n">
-        <v>0.00486</v>
+        <v>0.00203</v>
       </c>
       <c r="FY2" t="n">
-        <v>0.00702</v>
+        <v>0.00317</v>
       </c>
       <c r="FZ2" t="n">
-        <v>0.00685</v>
+        <v>0.00535</v>
       </c>
       <c r="GA2" t="n">
-        <v>0.01963</v>
+        <v>0.01174</v>
       </c>
       <c r="GB2" t="n">
-        <v>0.01464</v>
+        <v>0.01373</v>
       </c>
       <c r="GC2" t="n">
+        <v>0.00046</v>
+      </c>
+      <c r="GD2" t="n">
+        <v>0.00647</v>
+      </c>
+      <c r="GE2" t="n">
+        <v>0.00245</v>
+      </c>
+      <c r="GF2" t="n">
+        <v>0.00401</v>
+      </c>
+      <c r="GG2" t="n">
+        <v>0.0028</v>
+      </c>
+      <c r="GH2" t="n">
+        <v>0.00094</v>
+      </c>
+      <c r="GI2" t="n">
+        <v>0.00651</v>
+      </c>
+      <c r="GJ2" t="n">
+        <v>0.00358</v>
+      </c>
+      <c r="GK2" t="n">
+        <v>0.00417</v>
+      </c>
+      <c r="GL2" t="n">
+        <v>0.00497</v>
+      </c>
+      <c r="GM2" t="n">
+        <v>0.00305</v>
+      </c>
+      <c r="GN2" t="n">
+        <v>0.00412</v>
+      </c>
+      <c r="GO2" t="n">
+        <v>0.00724</v>
+      </c>
+      <c r="GP2" t="n">
+        <v>0.00159</v>
+      </c>
+      <c r="GQ2" t="n">
+        <v>0.00387</v>
+      </c>
+      <c r="GR2" t="n">
+        <v>0.00266</v>
+      </c>
+      <c r="GS2" t="n">
+        <v>0.00508</v>
+      </c>
+      <c r="GT2" t="n">
+        <v>0.00569</v>
+      </c>
+      <c r="GU2" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="GV2" t="n">
         <v>0.0025</v>
       </c>
-      <c r="GD2" t="n">
-        <v>0.008189999999999999</v>
-      </c>
-      <c r="GE2" t="n">
-        <v>0.00623</v>
-      </c>
-      <c r="GF2" t="n">
-        <v>0.00399</v>
-      </c>
-      <c r="GG2" t="n">
-        <v>0.00274</v>
-      </c>
-      <c r="GH2" t="n">
-        <v>0.01839</v>
-      </c>
-      <c r="GI2" t="n">
-        <v>0.01072</v>
-      </c>
-      <c r="GJ2" t="n">
+      <c r="GW2" t="n">
+        <v>0.00332</v>
+      </c>
+      <c r="GX2" t="n">
+        <v>0.00471</v>
+      </c>
+      <c r="GY2" t="n">
+        <v>0.00308</v>
+      </c>
+      <c r="GZ2" t="n">
+        <v>0.00123</v>
+      </c>
+      <c r="HA2" t="n">
+        <v>0.00708</v>
+      </c>
+      <c r="HB2" t="n">
+        <v>0.00443</v>
+      </c>
+      <c r="HC2" t="n">
+        <v>0.01147</v>
+      </c>
+      <c r="HD2" t="n">
+        <v>0.00299</v>
+      </c>
+      <c r="HE2" t="n">
+        <v>0.00328</v>
+      </c>
+      <c r="HF2" t="n">
+        <v>0.00452</v>
+      </c>
+      <c r="HG2" t="n">
+        <v>0.00105</v>
+      </c>
+      <c r="HH2" t="n">
         <v>0.00402</v>
       </c>
-      <c r="GK2" t="n">
-        <v>0.00659</v>
-      </c>
-      <c r="GL2" t="n">
-        <v>0.00453</v>
-      </c>
-      <c r="GM2" t="n">
-        <v>0.00479</v>
-      </c>
-      <c r="GN2" t="n">
-        <v>0.0072</v>
-      </c>
-      <c r="GO2" t="n">
-        <v>0.008750000000000001</v>
-      </c>
-      <c r="GP2" t="n">
-        <v>0.00197</v>
-      </c>
-      <c r="GQ2" t="n">
-        <v>0.00838</v>
-      </c>
-      <c r="GR2" t="n">
-        <v>0.00609</v>
-      </c>
-      <c r="GS2" t="n">
-        <v>0.01121</v>
-      </c>
-      <c r="GT2" t="n">
-        <v>0.00698</v>
-      </c>
-      <c r="GU2" t="n">
-        <v>0.00436</v>
-      </c>
-      <c r="GV2" t="n">
-        <v>0.0083</v>
-      </c>
-      <c r="GW2" t="n">
-        <v>0.00718</v>
-      </c>
-      <c r="GX2" t="n">
-        <v>0.00747</v>
-      </c>
-      <c r="GY2" t="n">
-        <v>0.00452</v>
-      </c>
-      <c r="GZ2" t="n">
-        <v>0.00339</v>
-      </c>
-      <c r="HA2" t="n">
-        <v>0.00392</v>
-      </c>
-      <c r="HB2" t="n">
-        <v>0.00373</v>
-      </c>
-      <c r="HC2" t="n">
-        <v>0.01834</v>
-      </c>
-      <c r="HD2" t="n">
-        <v>0.00577</v>
-      </c>
-      <c r="HE2" t="n">
-        <v>0.00532</v>
-      </c>
-      <c r="HF2" t="n">
-        <v>0.00486</v>
-      </c>
-      <c r="HG2" t="n">
-        <v>0.00267</v>
-      </c>
-      <c r="HH2" t="n">
-        <v>0.00219</v>
-      </c>
       <c r="HI2" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.00052</v>
       </c>
       <c r="HJ2" t="n">
-        <v>0.00197</v>
+        <v>0.00126</v>
       </c>
       <c r="HK2" t="n">
-        <v>0.00508</v>
+        <v>0.00525</v>
       </c>
       <c r="HL2" t="n">
-        <v>0.00413</v>
+        <v>0.00272</v>
       </c>
       <c r="HM2" t="n">
-        <v>0.00102</v>
+        <v>0.00039</v>
       </c>
       <c r="HN2" t="n">
-        <v>0.00515</v>
+        <v>0.0027</v>
       </c>
       <c r="HO2" t="n">
-        <v>0.00281</v>
+        <v>0.0033</v>
       </c>
       <c r="HP2" t="n">
-        <v>0.00319</v>
+        <v>0.00246</v>
       </c>
       <c r="HQ2" t="n">
-        <v>0.08507000000000001</v>
+        <v>0.008789999999999999</v>
       </c>
       <c r="HR2" t="n">
-        <v>0.00244</v>
+        <v>0.00192</v>
       </c>
       <c r="HS2" t="n">
-        <v>0.00312</v>
+        <v>0.00211</v>
       </c>
       <c r="HT2" t="n">
-        <v>0.00149</v>
+        <v>0.00085</v>
       </c>
       <c r="HU2" t="n">
-        <v>0.00282</v>
+        <v>0.00283</v>
       </c>
       <c r="HV2" t="n">
-        <v>0.00193</v>
+        <v>0.00083</v>
       </c>
       <c r="HW2" t="n">
-        <v>0.00114</v>
+        <v>0.00065</v>
       </c>
       <c r="HX2" t="n">
-        <v>0.0031</v>
+        <v>0.0005</v>
       </c>
       <c r="HY2" t="n">
-        <v>0.0025</v>
+        <v>0.0047</v>
       </c>
       <c r="HZ2" t="n">
-        <v>0.00367</v>
+        <v>0.00167</v>
       </c>
       <c r="IA2" t="n">
-        <v>0.0021</v>
+        <v>0.00141</v>
       </c>
       <c r="IB2" t="n">
-        <v>0.00568</v>
+        <v>0.00326</v>
       </c>
       <c r="IC2" t="n">
-        <v>0.00492</v>
+        <v>0.00368</v>
       </c>
       <c r="ID2" t="n">
-        <v>0.00144</v>
+        <v>0.00248</v>
       </c>
       <c r="IE2" t="n">
-        <v>0.00622</v>
+        <v>0.00165</v>
       </c>
       <c r="IF2" t="n">
-        <v>0.0333</v>
+        <v>0.0017</v>
       </c>
       <c r="IG2" t="n">
-        <v>0.00254</v>
+        <v>0.00109</v>
       </c>
       <c r="IH2" t="n">
-        <v>0.00188</v>
+        <v>0.00079</v>
       </c>
       <c r="II2" t="n">
-        <v>0.0028</v>
+        <v>0.00181</v>
       </c>
       <c r="IJ2" t="n">
-        <v>0.0007</v>
+        <v>0.00034</v>
       </c>
       <c r="IK2" t="n">
-        <v>0.00203</v>
+        <v>0.00364</v>
       </c>
       <c r="IL2" t="n">
-        <v>0.00443</v>
+        <v>0.00416</v>
       </c>
       <c r="IM2" t="n">
-        <v>0.00498</v>
+        <v>0.00186</v>
       </c>
       <c r="IN2" t="n">
-        <v>0.00217</v>
+        <v>0.00136</v>
       </c>
       <c r="IO2" t="n">
-        <v>0.00501</v>
+        <v>0.00125</v>
       </c>
       <c r="IP2" t="n">
-        <v>0.00183</v>
+        <v>0.00148</v>
       </c>
       <c r="IQ2" t="n">
-        <v>0.0042</v>
+        <v>0.00231</v>
       </c>
       <c r="IR2" t="n">
-        <v>0.00152</v>
+        <v>0.0004</v>
       </c>
       <c r="IS2" t="n">
-        <v>0.0023</v>
+        <v>0.00091</v>
       </c>
       <c r="IT2" t="n">
-        <v>0.00169</v>
+        <v>0.00105</v>
       </c>
       <c r="IU2" t="n">
-        <v>0.00313</v>
+        <v>0.00148</v>
       </c>
       <c r="IV2" t="n">
-        <v>0.00191</v>
+        <v>0.00036</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>